<commit_message>
2 new file added
</commit_message>
<xml_diff>
--- a/one.xlsx
+++ b/one.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Category</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Add</t>
   </si>
   <si>
+    <t>SUM()</t>
+  </si>
+  <si>
     <t>Two</t>
   </si>
   <si>
@@ -46,16 +49,25 @@
     <t>Count</t>
   </si>
   <si>
+    <t>COUNT()</t>
+  </si>
+  <si>
     <t>Four</t>
   </si>
   <si>
     <t>Max</t>
   </si>
   <si>
+    <t>MAX()</t>
+  </si>
+  <si>
     <t>Five</t>
   </si>
   <si>
     <t>Min</t>
+  </si>
+  <si>
+    <t>MIN()</t>
   </si>
   <si>
     <t>Addition</t>
@@ -78,10 +90,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -99,9 +111,85 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -115,121 +203,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,8 +218,44 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,7 +288,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,181 +306,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,6 +517,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -526,11 +541,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,6 +582,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -576,21 +606,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -599,166 +614,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -774,9 +780,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -792,11 +795,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="7"/>
@@ -1141,155 +1141,167 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>100</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="2">
         <v>200</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <f>B2+B5+B6</f>
         <v>5900</v>
       </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
         <v>1500</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="2">
         <v>500</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="11">
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="10">
         <f>C3-C4</f>
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="5">
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
         <v>2000</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>200</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="10">
         <f>COUNT(C2:C6)</f>
         <v>5</v>
       </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="4">
         <v>5000</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>4000</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="E5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="10">
         <f>MAX(C3:C6)</f>
         <v>4000</v>
       </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="5" t="s">
-        <v>12</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="4">
         <v>800</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>2000</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="E6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="10">
         <f>MIN(C3:C6)</f>
         <v>200</v>
       </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="7">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6">
         <f>SUM(B2:B6)</f>
         <v>9400</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <f>SUM(C2:C6)</f>
         <v>6900</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2">
         <f>(B7-C7)</f>
         <v>2500</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2">
         <f>B7*C7</f>
         <v>64860000</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <f>C2*C4</f>
         <v>40000</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2">
         <f>AVERAGE(B3:B6)</f>
         <v>2325</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <f>AVERAGE(C3:C6)</f>
         <v>1675</v>
       </c>

</xml_diff>